<commit_message>
Use Hex code for color instead of Enum
</commit_message>
<xml_diff>
--- a/EZSpreadsheet.Tests/ExpectedFiles/ShoulFillCellWithColor.xlsx
+++ b/EZSpreadsheet.Tests/ExpectedFiles/ShoulFillCellWithColor.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" r:id="R9bd2596335354f9e"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sheet1" sheetId="1" r:id="R2f4e9f003f6a4dd2"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -16,7 +16,7 @@
   <x:fonts count="1">
     <x:font>
       <x:sz val="11"/>
-      <x:color indexed="0"/>
+      <x:color rgb="000000"/>
       <x:name val="Calibri"/>
     </x:font>
   </x:fonts>
@@ -29,28 +29,28 @@
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor indexed="5"/>
+        <x:fgColor rgb="ECFF00"/>
       </x:patternFill>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="solid">
-        <x:fgColor indexed="6"/>
+        <x:fgColor rgb="FF00EC"/>
       </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
     <x:border>
       <x:left style="none">
-        <x:color indexed="0"/>
+        <x:color rgb="000000"/>
       </x:left>
       <x:right style="none">
-        <x:color indexed="0"/>
+        <x:color rgb="000000"/>
       </x:right>
       <x:top style="none">
-        <x:color indexed="0"/>
+        <x:color rgb="000000"/>
       </x:top>
       <x:bottom style="none">
-        <x:color indexed="0"/>
+        <x:color rgb="000000"/>
       </x:bottom>
     </x:border>
   </x:borders>

</xml_diff>